<commit_message>
First set of experiment results ready. Started experiment section.
</commit_message>
<xml_diff>
--- a/SCFrameworkImpl/Results/Current Results/ChangeTaskRate_05-10240/SkewedTasks_2_GENERAL.xlsx
+++ b/SCFrameworkImpl/Results/Current Results/ChangeTaskRate_05-10240/SkewedTasks_2_GENERAL.xlsx
@@ -1422,11 +1422,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="260215424"/>
-        <c:axId val="260215816"/>
+        <c:axId val="308604568"/>
+        <c:axId val="308603784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="260215424"/>
+        <c:axId val="308604568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1472,7 +1472,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260215816"/>
+        <c:crossAx val="308603784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1480,7 +1480,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260215816"/>
+        <c:axId val="308603784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,7 +1531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260215424"/>
+        <c:crossAx val="308604568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2506,11 +2506,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="260216600"/>
-        <c:axId val="260216992"/>
+        <c:axId val="308609664"/>
+        <c:axId val="308603392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="260216600"/>
+        <c:axId val="308609664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2609,7 +2609,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260216992"/>
+        <c:crossAx val="308603392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2617,7 +2617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260216992"/>
+        <c:axId val="308603392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2724,7 +2724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260216600"/>
+        <c:crossAx val="308609664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17459,7 +17459,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H13"/>
+      <selection activeCell="B25" sqref="B25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>